<commit_message>
teacher class successful , course classes & per class duration added
</commit_message>
<xml_diff>
--- a/.idea/Routine.xlsx
+++ b/.idea/Routine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Serial</t>
   </si>
@@ -106,19 +106,16 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>8:30am-11:30am;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t>9:00am-12:0pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t>8:30am-1:00pm;2:00pm-5:00pm</t>
-  </si>
-  <si>
-    <t>8:30am-1:00pm</t>
-  </si>
-  <si>
-    <t>2:00pm-5:00pm</t>
+    <t>8.30-11.30;14.00-17.00</t>
+  </si>
+  <si>
+    <t>9.00-12.00;14.00-17.00</t>
+  </si>
+  <si>
+    <t>14.00-17.00</t>
+  </si>
+  <si>
+    <t>8.30-13.00</t>
   </si>
 </sst>
 </file>
@@ -559,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
@@ -635,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,19 +691,19 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
teachers free time variable added
</commit_message>
<xml_diff>
--- a/.idea/Routine.xlsx
+++ b/.idea/Routine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Serial</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>Teacher</t>
-  </si>
-  <si>
-    <t>Saturday</t>
   </si>
   <si>
     <t>Sunday</t>
@@ -630,23 +627,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.26953125" customWidth="1"/>
-    <col min="3" max="3" width="29.6328125" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
-    <col min="6" max="6" width="30.26953125" customWidth="1"/>
-    <col min="7" max="7" width="30.6328125" customWidth="1"/>
+    <col min="2" max="2" width="29.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" customWidth="1"/>
+    <col min="6" max="6" width="30.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -665,45 +661,42 @@
       <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
       <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
teacher free time hash calulated success
</commit_message>
<xml_diff>
--- a/.idea/Routine.xlsx
+++ b/.idea/Routine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>Serial</t>
   </si>
@@ -67,9 +67,6 @@
     <t>AI</t>
   </si>
   <si>
-    <t>CSE 3203</t>
-  </si>
-  <si>
     <t>CSE 1211 Section 1</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>MMR</t>
   </si>
   <si>
-    <t>CSE 1201</t>
-  </si>
-  <si>
     <t>CSE 1211 Section 2</t>
   </si>
   <si>
@@ -106,13 +100,16 @@
     <t>8.30-11.30;14.00-17.00</t>
   </si>
   <si>
-    <t>9.00-12.00;14.00-17.00</t>
-  </si>
-  <si>
     <t>14.00-17.00</t>
   </si>
   <si>
     <t>8.30-13.00</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>10.00-11.30;14.00-17.00</t>
   </si>
 </sst>
 </file>
@@ -436,7 +433,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,7 +551,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,30 +591,30 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -629,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -644,22 +641,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -667,36 +664,39 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
       <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>